<commit_message>
additions to backend functions, included data in data repo, added notebook using a combination of openCLsim and openTNsim
</commit_message>
<xml_diff>
--- a/notebooks/shiptype_database/fleet_NPRC.xlsx
+++ b/notebooks/shiptype_database/fleet_NPRC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projecten\[121074] DigiTwin Vaarwegen\digitaltwin-waterway\notebooks\shiptype_database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B37247-884A-4183-BA5C-C3405471656E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47C6D01-DB0A-4C18-9249-1568C223D270}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5142FA11-04AC-4F28-862F-83D1DA72D2BB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="87">
   <si>
     <t>Ship Name</t>
   </si>
@@ -289,6 +289,12 @@
   </si>
   <si>
     <t>J3</t>
+  </si>
+  <si>
+    <t>110-er</t>
+  </si>
+  <si>
+    <t>135-er</t>
   </si>
 </sst>
 </file>
@@ -668,22 +674,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A50B148A-FA3E-4321-B0B5-73D709458982}">
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -700,7 +706,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -717,7 +723,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -734,7 +740,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -751,7 +757,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -768,7 +774,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -785,7 +791,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -802,7 +808,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -819,7 +825,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -836,7 +842,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
@@ -853,7 +859,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
@@ -870,7 +876,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
@@ -887,7 +893,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
@@ -904,7 +910,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
@@ -921,7 +927,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>21</v>
       </c>
@@ -938,7 +944,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
@@ -955,7 +961,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
@@ -972,7 +978,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
@@ -989,7 +995,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>26</v>
       </c>
@@ -1006,7 +1012,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>27</v>
       </c>
@@ -1023,7 +1029,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>28</v>
       </c>
@@ -1040,7 +1046,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>29</v>
       </c>
@@ -1057,7 +1063,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>30</v>
       </c>
@@ -1074,7 +1080,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>31</v>
       </c>
@@ -1091,7 +1097,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>32</v>
       </c>
@@ -1108,7 +1114,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>33</v>
       </c>
@@ -1125,7 +1131,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>35</v>
       </c>
@@ -1142,7 +1148,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>36</v>
       </c>
@@ -1159,7 +1165,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>37</v>
       </c>
@@ -1176,7 +1182,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>38</v>
       </c>
@@ -1193,7 +1199,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -1210,7 +1216,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>40</v>
       </c>
@@ -1227,7 +1233,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>41</v>
       </c>
@@ -1244,7 +1250,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>42</v>
       </c>
@@ -1261,7 +1267,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>43</v>
       </c>
@@ -1278,7 +1284,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>44</v>
       </c>
@@ -1295,7 +1301,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>45</v>
       </c>
@@ -1312,7 +1318,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>46</v>
       </c>
@@ -1329,7 +1335,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>47</v>
       </c>
@@ -1346,7 +1352,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>48</v>
       </c>
@@ -1363,7 +1369,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>49</v>
       </c>
@@ -1380,7 +1386,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>50</v>
       </c>
@@ -1397,7 +1403,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>51</v>
       </c>
@@ -1414,7 +1420,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>52</v>
       </c>
@@ -1431,7 +1437,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>53</v>
       </c>
@@ -1448,7 +1454,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>6</v>
       </c>
@@ -1465,7 +1471,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>55</v>
       </c>
@@ -1482,7 +1488,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>56</v>
       </c>
@@ -1499,7 +1505,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>57</v>
       </c>
@@ -1516,7 +1522,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>58</v>
       </c>
@@ -1533,7 +1539,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>59</v>
       </c>
@@ -1550,7 +1556,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>60</v>
       </c>
@@ -1567,7 +1573,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>61</v>
       </c>
@@ -1584,7 +1590,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>62</v>
       </c>
@@ -1601,7 +1607,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>63</v>
       </c>
@@ -1618,7 +1624,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>64</v>
       </c>
@@ -1635,7 +1641,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>65</v>
       </c>
@@ -1652,7 +1658,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>66</v>
       </c>
@@ -1669,7 +1675,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>68</v>
       </c>
@@ -1686,7 +1692,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>69</v>
       </c>
@@ -1703,7 +1709,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>70</v>
       </c>
@@ -1720,7 +1726,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>9</v>
       </c>
@@ -1737,7 +1743,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>71</v>
       </c>
@@ -1754,7 +1760,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>72</v>
       </c>
@@ -1771,7 +1777,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>73</v>
       </c>
@@ -1788,7 +1794,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>74</v>
       </c>
@@ -1805,7 +1811,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>75</v>
       </c>
@@ -1822,7 +1828,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>76</v>
       </c>
@@ -1839,7 +1845,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>77</v>
       </c>
@@ -1856,7 +1862,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>78</v>
       </c>
@@ -1873,7 +1879,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>80</v>
       </c>
@@ -1890,7 +1896,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>81</v>
       </c>
@@ -1907,7 +1913,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>82</v>
       </c>
@@ -1924,7 +1930,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>83</v>
       </c>
@@ -1941,7 +1947,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>84</v>
       </c>
@@ -1955,6 +1961,40 @@
         <v>3950</v>
       </c>
       <c r="E75" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B76">
+        <v>11.5</v>
+      </c>
+      <c r="C76">
+        <v>110</v>
+      </c>
+      <c r="D76">
+        <v>3000</v>
+      </c>
+      <c r="E76" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B77">
+        <v>11.5</v>
+      </c>
+      <c r="C77">
+        <v>135</v>
+      </c>
+      <c r="D77">
+        <v>4000</v>
+      </c>
+      <c r="E77" t="s">
         <v>79</v>
       </c>
     </row>

</xml_diff>